<commit_message>
Commit enhancements to AnalyzeNetworkPointFlow.  Command works as documented.
git-svn-id: file:///cygdrive/C/owf-svnrepos/TSTool-test/java_142/trunk@889 fa08ced2-b08f-4ccc-859c-2e92e4a1381a
</commit_message>
<xml_diff>
--- a/test/regression/commands/general/AnalyzeNetworkPointFlow/Data/Network1.xlsx
+++ b/test/regression/commands/general/AnalyzeNetworkPointFlow/Data/Network1.xlsx
@@ -597,7 +597,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +849,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" s="10">
         <v>3</v>
@@ -870,7 +870,7 @@
         <v>41</v>
       </c>
       <c r="D13" s="10">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E13" s="10">
         <v>4</v>
@@ -891,7 +891,7 @@
         <v>41</v>
       </c>
       <c r="D14" s="10">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E14" s="10">
         <v>4</v>
@@ -912,7 +912,7 @@
         <v>40</v>
       </c>
       <c r="D15" s="10">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E15" s="10">
         <v>4</v>
@@ -933,7 +933,7 @@
         <v>41</v>
       </c>
       <c r="D16" s="10">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E16" s="10">
         <v>4</v>
@@ -954,7 +954,7 @@
         <v>41</v>
       </c>
       <c r="D17" s="10">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E17" s="10">
         <v>5</v>
@@ -975,7 +975,7 @@
         <v>41</v>
       </c>
       <c r="D18" s="10">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E18" s="10">
         <v>5</v>
@@ -996,7 +996,7 @@
         <v>41</v>
       </c>
       <c r="D19" s="10">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="E19" s="10">
         <v>5</v>
@@ -1017,7 +1017,7 @@
         <v>40</v>
       </c>
       <c r="D20" s="10">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E20" s="10">
         <v>5</v>

</xml_diff>